<commit_message>
added demand reactions to table S1
</commit_message>
<xml_diff>
--- a/results/tables/table_S1.xlsx
+++ b/results/tables/table_S1.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GENRE Topology Breakdown" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Additional Comparison Metrics" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AGORA model demand reactions" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="100">
   <si>
     <t xml:space="preserve">GENRE name:</t>
   </si>
@@ -189,6 +190,138 @@
   </si>
   <si>
     <t xml:space="preserve">agora_R20291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGORA str. NAP07 GENRE demand reactions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_4HBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink needed to allow 4-hydroxy-benzoate to leave system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_HQN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink needed to allow Hydroquinone to leave system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_btn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand for biotin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpn140(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (tetratetradecanoyl, n-C14:0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpn160(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (tetrahexadecanoyl, n-C16:0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpn180(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (tetraoctadecanoyl, n-C18:0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpni16(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (14-methyl-pentadecanoyl, iso-C16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_dhptd(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand reaction for 4,5-dihydroxy-2,3-pentanedione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sink_dmbzid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink for 5,6-Dimenthylbenzimidazole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGORA str. NAP08 demand reactions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGORA str. CD196 GENRE demand reactions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_5DRIB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink needed to allow 5-deoxyribose to leave system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_5MTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink needed to allow 5-Methylthio-D-ribose to leave system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_GCALD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink needed to allow glycol aldehyde to leave system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpnai15(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (12-methyl-tetradecanoyl, anteiso-C15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpnai17(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (14-methyl-hexadecanoyl, anteiso-C17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpni15(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (13-methyl-tetradecanoyl, iso-C15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_clpni17(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for cardiolipin (15-methyl-hexadecanoyl, iso-C17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_dad_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand for 5-deoxyadenosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM_teich_45_BS(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand reaction for teichuronic acid (GlcA + GalNac, 45 repeating unit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sink_PGPm1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sink reaction for peptidoglycan polymer (n-1) subunits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sink_gthrd(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sink reaction for reduced glutathione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGORA str. R20291 GENRE demand reactions:</t>
   </si>
 </sst>
 </file>
@@ -282,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,6 +480,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +503,7 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -979,7 +1116,7 @@
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -1661,4 +1798,526 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D64"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A45:D45"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>